<commit_message>
modif description HS sensitive unit 40566b065f262ff3b70c374eccadeb3cf288b0c4
</commit_message>
<xml_diff>
--- a/sd-change-def-ror-healthcareservice-sensitive-unit/ig/StructureDefinition-ror-healthcareservice-sensitive-unit.xlsx
+++ b/sd-change-def-ror-healthcareservice-sensitive-unit/ig/StructureDefinition-ror-healthcareservice-sensitive-unit.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-13T15:33:31+00:00</t>
+    <t>2024-06-13T16:28:56+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -78,7 +78,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Extension créée dans le cadre du ROR pour signaler que toutes les informations de description d'une offre sont confidentielles car elles présentent un risque d'utilisation à des fins malveillantes.</t>
+    <t>Extension créée dans le cadre du ROR pour signaler que toutes les informations de description d'une offre sont confidentielles car elles présentent un risque d'utilisation à des fins malveillantes, ou que le porteur d'offre ne souhaite pas diffuser.</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>